<commit_message>
fix(DTFS2-8124): accrual currency validation changed to ISO4217
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0AFF25-C101-495B-AAFC-97B709F5B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA11D4D-D308-4AF6-BE4F-C40EB419E04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>BHD</t>
+  </si>
+  <si>
+    <t>Accrual currency</t>
+  </si>
+  <si>
+    <t>accrual exchange rate</t>
+  </si>
+  <si>
+    <t>INRA</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +598,7 @@
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +632,14 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -655,8 +673,14 @@
       <c r="K2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>1.2230000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -690,8 +714,14 @@
       <c r="K3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -704,7 +734,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -716,7 +746,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -729,17 +759,17 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -752,7 +782,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -765,7 +795,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -778,14 +808,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -797,7 +827,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -810,7 +840,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
fix(DTFS2-8124): add invalid currency fixture
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0AFF25-C101-495B-AAFC-97B709F5B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D8D1F-A5AD-4F79-AF5A-A9D4E3BFD776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>BHD</t>
+  </si>
+  <si>
+    <t>Accrual currency</t>
+  </si>
+  <si>
+    <t>accrual exchange rate</t>
+  </si>
+  <si>
+    <t>INRA</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L1" sqref="L1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +598,7 @@
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +632,14 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -655,8 +673,14 @@
       <c r="K2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>1.2230000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -690,8 +714,14 @@
       <c r="K3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -704,7 +734,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -716,7 +746,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -729,17 +759,17 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -752,7 +782,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -765,7 +795,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -778,14 +808,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -797,7 +827,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -810,7 +840,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
fix(DTFS2-8124): e2etf - accrual currency validation changed to ISO4217 (#4429)
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0AFF25-C101-495B-AAFC-97B709F5B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D8D1F-A5AD-4F79-AF5A-A9D4E3BFD776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>BHD</t>
+  </si>
+  <si>
+    <t>Accrual currency</t>
+  </si>
+  <si>
+    <t>accrual exchange rate</t>
+  </si>
+  <si>
+    <t>INRA</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L1" sqref="L1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +598,7 @@
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +632,14 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -655,8 +673,14 @@
       <c r="K2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>1.2230000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -690,8 +714,14 @@
       <c r="K3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -704,7 +734,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -716,7 +746,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -729,17 +759,17 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -752,7 +782,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -765,7 +795,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -778,14 +808,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -797,7 +827,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -810,7 +840,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
chore(merge): merge release-2.10.0 to main (#4434)
Co-authored-by: Abhi Markan <amarkan>
Co-authored-by: zainUKEF <zain.kassam@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/invalid-utilisation-report-February_2023_monthly-invalid-currencies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZKassam\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0AFF25-C101-495B-AAFC-97B709F5B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D8D1F-A5AD-4F79-AF5A-A9D4E3BFD776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>BHD</t>
+  </si>
+  <si>
+    <t>Accrual currency</t>
+  </si>
+  <si>
+    <t>accrual exchange rate</t>
+  </si>
+  <si>
+    <t>INRA</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132C8B60-A9FF-47A2-964A-EAE307991DDE}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L1" sqref="L1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +598,7 @@
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +632,14 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -655,8 +673,14 @@
       <c r="K2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>1.2230000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -690,8 +714,14 @@
       <c r="K3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -704,7 +734,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -716,7 +746,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -729,17 +759,17 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -752,7 +782,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -765,7 +795,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -778,14 +808,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -797,7 +827,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -810,7 +840,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>

</xml_diff>